<commit_message>
gen new data format
</commit_message>
<xml_diff>
--- a/result_data/全新实验数据.xlsx
+++ b/result_data/全新实验数据.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Helen/Documents/Mphi/TOSN/TOSN_helen_copy3/result_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D7E38F-5096-5842-93AD-B0F4BAB37E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF1F6F-AD82-2E4B-A113-420652DB0A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{5C3BF085-E378-EC45-A4E0-3E9E9423F4C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>pattern 实验</t>
   </si>
@@ -56,23 +56,51 @@
     <t>ours</t>
   </si>
   <si>
-    <t>100%的数据为 norm~</t>
-  </si>
-  <si>
-    <t>50%的数据为 norm~ 500ep</t>
-  </si>
-  <si>
-    <t>70%的数据为 norm 1100ep</t>
-  </si>
-  <si>
-    <t>50%的数据为 norm~ 1100ep</t>
+    <t>50%的数据为 norm 1100ep</t>
+  </si>
+  <si>
+    <t>25%的数据为 norm 1100ep</t>
+  </si>
+  <si>
+    <t>0%的数据为 norm 1100ep</t>
+  </si>
+  <si>
+    <t>正态分布细分实验</t>
+  </si>
+  <si>
+    <t>根据时间变化的task平均cost实验</t>
+  </si>
+  <si>
+    <t>sigma,mu全随机</t>
+  </si>
+  <si>
+    <t>100%的数据为 norm~ 1100ep</t>
+  </si>
+  <si>
+    <t>75%的数据为 norm 1100ep</t>
+  </si>
+  <si>
+    <t>单峰值，sigma</t>
+  </si>
+  <si>
+    <t>ours reward</t>
+  </si>
+  <si>
+    <t>ppo  reward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,10 +138,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,13 +150,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,19 +477,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3C281F-F2B6-044D-A78B-8F6E3013861B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="27.83203125" customWidth="1"/>
+    <col min="4" max="5" width="30.1640625" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,62 +499,167 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-4129.2460000000001</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-3984.9670000000001</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-4741.6120000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-4930.1090000000004</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-4613.7719999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-3651.8580000000002</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-3548.7489999999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-4579.5240000000003</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-4888.6019999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-4314.3530000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="8">
+        <f>(B7-B6)/-B6</f>
+        <v>0.11561142155250617</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" ref="C8:F8" si="0">(C7-C6)/-C6</f>
+        <v>0.10946590021950001</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>3.4184155093246717E-2</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>8.4190836348649722E-3</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>6.4896791605653661E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>24.078073430170001</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>21.903391691426101</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>